<commit_message>
Day1 + 2 updated
</commit_message>
<xml_diff>
--- a/Python/UDEMY-100 Days of Code/Resources/100_Days_of_Code_Walkthrough.xlsx
+++ b/Python/UDEMY-100 Days of Code/Resources/100_Days_of_Code_Walkthrough.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanja\Desktop\Github 2025\Programming-Languages\Python\UDEMY-100 Days of Code\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C49D7A-A82D-4BFF-8B6D-28479604BF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D2DCD2-CF40-4FC4-BDE5-1EC7DFFDC23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E9612FF2-2173-4D37-B82C-2AE8BC909B02}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E9612FF2-2173-4D37-B82C-2AE8BC909B02}"/>
   </bookViews>
   <sheets>
     <sheet name="1-Beginner" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Day</t>
   </si>
@@ -73,6 +73,25 @@
   </si>
   <si>
     <t>1. Band Name Generator</t>
+  </si>
+  <si>
+    <t>Understanding Data Types and How to Manipulate Strings</t>
+  </si>
+  <si>
+    <t>1. Data Types - Type Error, Strings, Integer, Float, Boolean
+2. Type function, checking, conversion
+3. Number Manipulation
+4. f-Strings</t>
+  </si>
+  <si>
+    <t>2. Data Types Quiz
+3. Mathematical Operations Quiz</t>
+  </si>
+  <si>
+    <t>https://docs.python.org/3/tutorial/floatingpoint.html</t>
+  </si>
+  <si>
+    <t>2. Tip Calculator</t>
   </si>
 </sst>
 </file>
@@ -472,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F59A2EF-40CB-4966-A77C-1DC74EC78C0F}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,9 +546,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{A3C2C91A-8874-4C52-92FB-16FDCB176E32}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{A45A563E-E70F-4285-B56C-8DC8E4B04082}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>